<commit_message>
them xoa sua voucher
</commit_message>
<xml_diff>
--- a/sanpham.xlsx
+++ b/sanpham.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Mã sản phẩm</t>
   </si>
@@ -36,24 +36,6 @@
   </si>
   <si>
     <t>Còn hàng</t>
-  </si>
-  <si>
-    <t>Tu dien</t>
-  </si>
-  <si>
-    <t>Nguyen Chi Vinh</t>
-  </si>
-  <si>
-    <t>Sach giao khoa</t>
-  </si>
-  <si>
-    <t>Người thầy</t>
-  </si>
-  <si>
-    <t>Truyen vui</t>
-  </si>
-  <si>
-    <t>Truyen</t>
   </si>
 </sst>
 </file>
@@ -149,7 +131,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -157,10 +139,10 @@
   <cols>
     <col min="1" max="1" width="12.0546875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.3828125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.16015625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.83203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="4.9296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.13671875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="6.5625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="7.42578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="3.6640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="8.25390625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="6.71875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="8.5859375" customWidth="true" bestFit="true"/>
   </cols>
@@ -191,84 +173,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>8.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>7000.0</v>
-      </c>
-      <c r="F2" t="n" s="1">
-        <v>45571.0</v>
-      </c>
-      <c r="G2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H2" t="n" s="0">
-        <v>500.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>7000.0</v>
-      </c>
-      <c r="F3" t="n" s="1">
-        <v>45571.0</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>18.0</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>500.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>1000.0</v>
-      </c>
-      <c r="F4" t="n" s="1">
-        <v>45571.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>500.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>